<commit_message>
more test data generation stuff
</commit_message>
<xml_diff>
--- a/test_data/generate_sql.xlsx
+++ b/test_data/generate_sql.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="receiving_locations" sheetId="1" r:id="rId1"/>
     <sheet name="stocking_purchase_orders" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="24">
   <si>
     <t>status</t>
   </si>
@@ -56,6 +57,42 @@
   </si>
   <si>
     <t>Requested</t>
+  </si>
+  <si>
+    <t>temperature_zone</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>dry'::temperature_zone</t>
+  </si>
+  <si>
+    <t>Pallet Storage'::stocking_location_type</t>
+  </si>
+  <si>
+    <t>pick_segment</t>
+  </si>
+  <si>
+    <t>aisle</t>
+  </si>
+  <si>
+    <t>bay</t>
+  </si>
+  <si>
+    <t>shelf</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>depth</t>
   </si>
 </sst>
 </file>
@@ -104,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -136,12 +173,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -157,6 +245,31 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -172,6 +285,31 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,9 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -977,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -1376,4 +1512,3807 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>204168900281</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>48</v>
+      </c>
+      <c r="J2">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <v>48</v>
+      </c>
+      <c r="L2" t="str">
+        <f>CONCATENATE("insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('", A2, "?', '", B2, ", '", C2, ", ", D2, ", ", E2, ", ", F2, ", ", G2, ", ", H2, ", ", I2, ", ", J2, ", ", K2, ");")</f>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900281?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>204168900282</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>48</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L66" si="0">CONCATENATE("insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('", A3, "?', '", B3, ", '", C3, ", ", D3, ", ", E3, ", ", F3, ", ", G3, ", ", H3, ", ", I3, ", ", J3, ", ", K3, ");")</f>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900282?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>204168900283</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>48</v>
+      </c>
+      <c r="J4">
+        <v>48</v>
+      </c>
+      <c r="K4">
+        <v>48</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900283?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>204168900284</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>48</v>
+      </c>
+      <c r="J5">
+        <v>48</v>
+      </c>
+      <c r="K5">
+        <v>48</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900284?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>204168900285</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>48</v>
+      </c>
+      <c r="J6">
+        <v>48</v>
+      </c>
+      <c r="K6">
+        <v>48</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900285?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>204168900286</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>48</v>
+      </c>
+      <c r="J7">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <v>48</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900286?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 1, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>204168900287</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>48</v>
+      </c>
+      <c r="J8">
+        <v>48</v>
+      </c>
+      <c r="K8">
+        <v>48</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900287?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>204168900288</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>48</v>
+      </c>
+      <c r="J9">
+        <v>48</v>
+      </c>
+      <c r="K9">
+        <v>48</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900288?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>204168900289</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>48</v>
+      </c>
+      <c r="J10">
+        <v>48</v>
+      </c>
+      <c r="K10">
+        <v>48</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900289?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>204168900290</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>48</v>
+      </c>
+      <c r="J11">
+        <v>48</v>
+      </c>
+      <c r="K11">
+        <v>48</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900290?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>204168900291</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>48</v>
+      </c>
+      <c r="J12">
+        <v>48</v>
+      </c>
+      <c r="K12">
+        <v>48</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900291?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>204168900292</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>48</v>
+      </c>
+      <c r="J13">
+        <v>48</v>
+      </c>
+      <c r="K13">
+        <v>48</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900292?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 2, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>204168900293</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>48</v>
+      </c>
+      <c r="J14">
+        <v>48</v>
+      </c>
+      <c r="K14">
+        <v>48</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900293?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>204168900294</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>48</v>
+      </c>
+      <c r="J15">
+        <v>48</v>
+      </c>
+      <c r="K15">
+        <v>48</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900294?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>204168900295</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="J16">
+        <v>48</v>
+      </c>
+      <c r="K16">
+        <v>48</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900295?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>204168900296</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>48</v>
+      </c>
+      <c r="J17">
+        <v>48</v>
+      </c>
+      <c r="K17">
+        <v>48</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900296?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>204168900297</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>48</v>
+      </c>
+      <c r="J18">
+        <v>48</v>
+      </c>
+      <c r="K18">
+        <v>48</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900297?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>204168900298</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>48</v>
+      </c>
+      <c r="J19">
+        <v>48</v>
+      </c>
+      <c r="K19">
+        <v>48</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900298?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 3, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>204168900299</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>48</v>
+      </c>
+      <c r="J20">
+        <v>48</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900299?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>204168900300</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>48</v>
+      </c>
+      <c r="J21">
+        <v>48</v>
+      </c>
+      <c r="K21">
+        <v>48</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900300?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>204168900301</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>48</v>
+      </c>
+      <c r="J22">
+        <v>48</v>
+      </c>
+      <c r="K22">
+        <v>48</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900301?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>204168900302</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>48</v>
+      </c>
+      <c r="J23">
+        <v>48</v>
+      </c>
+      <c r="K23">
+        <v>48</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900302?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>204168900303</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>48</v>
+      </c>
+      <c r="J24">
+        <v>48</v>
+      </c>
+      <c r="K24">
+        <v>48</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900303?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>204168900304</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>48</v>
+      </c>
+      <c r="J25">
+        <v>48</v>
+      </c>
+      <c r="K25">
+        <v>48</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900304?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 1, 4, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>204168900305</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>48</v>
+      </c>
+      <c r="J26">
+        <v>48</v>
+      </c>
+      <c r="K26">
+        <v>48</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900305?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>204168900306</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>48</v>
+      </c>
+      <c r="J27">
+        <v>48</v>
+      </c>
+      <c r="K27">
+        <v>48</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900306?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>204168900307</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>48</v>
+      </c>
+      <c r="J28">
+        <v>48</v>
+      </c>
+      <c r="K28">
+        <v>48</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900307?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>204168900308</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>48</v>
+      </c>
+      <c r="J29">
+        <v>48</v>
+      </c>
+      <c r="K29">
+        <v>48</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900308?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>204168900309</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>48</v>
+      </c>
+      <c r="J30">
+        <v>48</v>
+      </c>
+      <c r="K30">
+        <v>48</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900309?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>204168900310</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>48</v>
+      </c>
+      <c r="J31">
+        <v>48</v>
+      </c>
+      <c r="K31">
+        <v>48</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900310?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 5, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>204168900311</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>48</v>
+      </c>
+      <c r="J32">
+        <v>48</v>
+      </c>
+      <c r="K32">
+        <v>48</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900311?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>204168900312</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>48</v>
+      </c>
+      <c r="J33">
+        <v>48</v>
+      </c>
+      <c r="K33">
+        <v>48</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900312?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>204168900313</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>48</v>
+      </c>
+      <c r="J34">
+        <v>48</v>
+      </c>
+      <c r="K34">
+        <v>48</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900313?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>204168900314</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>48</v>
+      </c>
+      <c r="J35">
+        <v>48</v>
+      </c>
+      <c r="K35">
+        <v>48</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900314?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>204168900315</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>48</v>
+      </c>
+      <c r="J36">
+        <v>48</v>
+      </c>
+      <c r="K36">
+        <v>48</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900315?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>204168900316</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>48</v>
+      </c>
+      <c r="J37">
+        <v>48</v>
+      </c>
+      <c r="K37">
+        <v>48</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900316?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 6, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>204168900317</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>48</v>
+      </c>
+      <c r="J38">
+        <v>48</v>
+      </c>
+      <c r="K38">
+        <v>48</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900317?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>204168900318</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>7</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>48</v>
+      </c>
+      <c r="J39">
+        <v>48</v>
+      </c>
+      <c r="K39">
+        <v>48</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900318?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>204168900319</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>48</v>
+      </c>
+      <c r="J40">
+        <v>48</v>
+      </c>
+      <c r="K40">
+        <v>48</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900319?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>204168900320</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>48</v>
+      </c>
+      <c r="J41">
+        <v>48</v>
+      </c>
+      <c r="K41">
+        <v>48</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900320?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>204168900321</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>48</v>
+      </c>
+      <c r="J42">
+        <v>48</v>
+      </c>
+      <c r="K42">
+        <v>48</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900321?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>204168900322</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>48</v>
+      </c>
+      <c r="J43">
+        <v>48</v>
+      </c>
+      <c r="K43">
+        <v>48</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900322?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 7, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>204168900323</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>48</v>
+      </c>
+      <c r="J44">
+        <v>48</v>
+      </c>
+      <c r="K44">
+        <v>48</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900323?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>204168900324</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>48</v>
+      </c>
+      <c r="J45">
+        <v>48</v>
+      </c>
+      <c r="K45">
+        <v>48</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900324?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>204168900325</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>48</v>
+      </c>
+      <c r="J46">
+        <v>48</v>
+      </c>
+      <c r="K46">
+        <v>48</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900325?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>204168900326</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>48</v>
+      </c>
+      <c r="J47">
+        <v>48</v>
+      </c>
+      <c r="K47">
+        <v>48</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900326?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>204168900327</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>48</v>
+      </c>
+      <c r="J48">
+        <v>48</v>
+      </c>
+      <c r="K48">
+        <v>48</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900327?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>204168900328</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>8</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>48</v>
+      </c>
+      <c r="J49">
+        <v>48</v>
+      </c>
+      <c r="K49">
+        <v>48</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900328?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 1, 8, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>204168900329</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>48</v>
+      </c>
+      <c r="J50">
+        <v>48</v>
+      </c>
+      <c r="K50">
+        <v>48</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900329?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>204168900330</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>48</v>
+      </c>
+      <c r="J51">
+        <v>48</v>
+      </c>
+      <c r="K51">
+        <v>48</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900330?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>204168900331</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>48</v>
+      </c>
+      <c r="J52">
+        <v>48</v>
+      </c>
+      <c r="K52">
+        <v>48</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900331?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>204168900332</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>48</v>
+      </c>
+      <c r="J53">
+        <v>48</v>
+      </c>
+      <c r="K53">
+        <v>48</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900332?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54">
+        <v>204168900333</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>48</v>
+      </c>
+      <c r="J54">
+        <v>48</v>
+      </c>
+      <c r="K54">
+        <v>48</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900333?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55">
+        <v>204168900334</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>48</v>
+      </c>
+      <c r="J55">
+        <v>48</v>
+      </c>
+      <c r="K55">
+        <v>48</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900334?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 1, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56">
+        <v>204168900335</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>48</v>
+      </c>
+      <c r="J56">
+        <v>48</v>
+      </c>
+      <c r="K56">
+        <v>48</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900335?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57">
+        <v>204168900336</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>48</v>
+      </c>
+      <c r="J57">
+        <v>48</v>
+      </c>
+      <c r="K57">
+        <v>48</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900336?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>204168900337</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>48</v>
+      </c>
+      <c r="J58">
+        <v>48</v>
+      </c>
+      <c r="K58">
+        <v>48</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900337?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>204168900338</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>48</v>
+      </c>
+      <c r="J59">
+        <v>48</v>
+      </c>
+      <c r="K59">
+        <v>48</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900338?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>204168900339</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>48</v>
+      </c>
+      <c r="J60">
+        <v>48</v>
+      </c>
+      <c r="K60">
+        <v>48</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900339?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>204168900340</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <v>48</v>
+      </c>
+      <c r="J61">
+        <v>48</v>
+      </c>
+      <c r="K61">
+        <v>48</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900340?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 2, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>204168900341</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>48</v>
+      </c>
+      <c r="J62">
+        <v>48</v>
+      </c>
+      <c r="K62">
+        <v>48</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900341?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>204168900342</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>48</v>
+      </c>
+      <c r="J63">
+        <v>48</v>
+      </c>
+      <c r="K63">
+        <v>48</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900342?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>204168900343</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>48</v>
+      </c>
+      <c r="J64">
+        <v>48</v>
+      </c>
+      <c r="K64">
+        <v>48</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900343?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>204168900344</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65">
+        <v>48</v>
+      </c>
+      <c r="J65">
+        <v>48</v>
+      </c>
+      <c r="K65">
+        <v>48</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900344?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>204168900345</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>48</v>
+      </c>
+      <c r="J66">
+        <v>48</v>
+      </c>
+      <c r="K66">
+        <v>48</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900345?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>204168900346</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>48</v>
+      </c>
+      <c r="J67">
+        <v>48</v>
+      </c>
+      <c r="K67">
+        <v>48</v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L97" si="1">CONCATENATE("insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('", A67, "?', '", B67, ", '", C67, ", ", D67, ", ", E67, ", ", F67, ", ", G67, ", ", H67, ", ", I67, ", ", J67, ", ", K67, ");")</f>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900346?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 3, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68">
+        <v>204168900347</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>4</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>48</v>
+      </c>
+      <c r="J68">
+        <v>48</v>
+      </c>
+      <c r="K68">
+        <v>48</v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900347?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69">
+        <v>204168900348</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>48</v>
+      </c>
+      <c r="J69">
+        <v>48</v>
+      </c>
+      <c r="K69">
+        <v>48</v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900348?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70">
+        <v>204168900349</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>4</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>48</v>
+      </c>
+      <c r="J70">
+        <v>48</v>
+      </c>
+      <c r="K70">
+        <v>48</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900349?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71">
+        <v>204168900350</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <v>4</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>48</v>
+      </c>
+      <c r="J71">
+        <v>48</v>
+      </c>
+      <c r="K71">
+        <v>48</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900350?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72">
+        <v>204168900351</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>48</v>
+      </c>
+      <c r="J72">
+        <v>48</v>
+      </c>
+      <c r="K72">
+        <v>48</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900351?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73">
+        <v>204168900352</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>48</v>
+      </c>
+      <c r="J73">
+        <v>48</v>
+      </c>
+      <c r="K73">
+        <v>48</v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900352?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 1, 2, 4, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74">
+        <v>204168900353</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>48</v>
+      </c>
+      <c r="J74">
+        <v>48</v>
+      </c>
+      <c r="K74">
+        <v>48</v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900353?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75">
+        <v>204168900354</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>5</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="I75">
+        <v>48</v>
+      </c>
+      <c r="J75">
+        <v>48</v>
+      </c>
+      <c r="K75">
+        <v>48</v>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900354?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76">
+        <v>204168900355</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>5</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>48</v>
+      </c>
+      <c r="J76">
+        <v>48</v>
+      </c>
+      <c r="K76">
+        <v>48</v>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900355?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77">
+        <v>204168900356</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>48</v>
+      </c>
+      <c r="J77">
+        <v>48</v>
+      </c>
+      <c r="K77">
+        <v>48</v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900356?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78">
+        <v>204168900357</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>5</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>48</v>
+      </c>
+      <c r="J78">
+        <v>48</v>
+      </c>
+      <c r="K78">
+        <v>48</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900357?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79">
+        <v>204168900358</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>2</v>
+      </c>
+      <c r="I79">
+        <v>48</v>
+      </c>
+      <c r="J79">
+        <v>48</v>
+      </c>
+      <c r="K79">
+        <v>48</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900358?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 5, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80">
+        <v>204168900359</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>6</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>48</v>
+      </c>
+      <c r="J80">
+        <v>48</v>
+      </c>
+      <c r="K80">
+        <v>48</v>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900359?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81">
+        <v>204168900360</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>6</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="I81">
+        <v>48</v>
+      </c>
+      <c r="J81">
+        <v>48</v>
+      </c>
+      <c r="K81">
+        <v>48</v>
+      </c>
+      <c r="L81" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900360?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82">
+        <v>204168900361</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>6</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>48</v>
+      </c>
+      <c r="J82">
+        <v>48</v>
+      </c>
+      <c r="K82">
+        <v>48</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900361?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83">
+        <v>204168900362</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>6</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83">
+        <v>48</v>
+      </c>
+      <c r="J83">
+        <v>48</v>
+      </c>
+      <c r="K83">
+        <v>48</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900362?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84">
+        <v>204168900363</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>6</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>48</v>
+      </c>
+      <c r="J84">
+        <v>48</v>
+      </c>
+      <c r="K84">
+        <v>48</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900363?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85">
+        <v>204168900364</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>6</v>
+      </c>
+      <c r="G85">
+        <v>3</v>
+      </c>
+      <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85">
+        <v>48</v>
+      </c>
+      <c r="J85">
+        <v>48</v>
+      </c>
+      <c r="K85">
+        <v>48</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900364?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 6, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
+        <v>204168900365</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86">
+        <v>7</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>48</v>
+      </c>
+      <c r="J86">
+        <v>48</v>
+      </c>
+      <c r="K86">
+        <v>48</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900365?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87">
+        <v>204168900366</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>7</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>2</v>
+      </c>
+      <c r="I87">
+        <v>48</v>
+      </c>
+      <c r="J87">
+        <v>48</v>
+      </c>
+      <c r="K87">
+        <v>48</v>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900366?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88">
+        <v>204168900367</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>7</v>
+      </c>
+      <c r="G88">
+        <v>2</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>48</v>
+      </c>
+      <c r="J88">
+        <v>48</v>
+      </c>
+      <c r="K88">
+        <v>48</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900367?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89">
+        <v>204168900368</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89">
+        <v>7</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89">
+        <v>2</v>
+      </c>
+      <c r="I89">
+        <v>48</v>
+      </c>
+      <c r="J89">
+        <v>48</v>
+      </c>
+      <c r="K89">
+        <v>48</v>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900368?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90">
+        <v>204168900369</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90">
+        <v>7</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>48</v>
+      </c>
+      <c r="J90">
+        <v>48</v>
+      </c>
+      <c r="K90">
+        <v>48</v>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900369?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91">
+        <v>204168900370</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>7</v>
+      </c>
+      <c r="G91">
+        <v>3</v>
+      </c>
+      <c r="H91">
+        <v>2</v>
+      </c>
+      <c r="I91">
+        <v>48</v>
+      </c>
+      <c r="J91">
+        <v>48</v>
+      </c>
+      <c r="K91">
+        <v>48</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900370?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 7, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92">
+        <v>204168900371</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>8</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>48</v>
+      </c>
+      <c r="J92">
+        <v>48</v>
+      </c>
+      <c r="K92">
+        <v>48</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900371?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 1, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93">
+        <v>204168900372</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>8</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>2</v>
+      </c>
+      <c r="I93">
+        <v>48</v>
+      </c>
+      <c r="J93">
+        <v>48</v>
+      </c>
+      <c r="K93">
+        <v>48</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900372?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 1, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94">
+        <v>204168900373</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>8</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>48</v>
+      </c>
+      <c r="J94">
+        <v>48</v>
+      </c>
+      <c r="K94">
+        <v>48</v>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900373?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 2, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95">
+        <v>204168900374</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <v>8</v>
+      </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
+      <c r="H95">
+        <v>2</v>
+      </c>
+      <c r="I95">
+        <v>48</v>
+      </c>
+      <c r="J95">
+        <v>48</v>
+      </c>
+      <c r="K95">
+        <v>48</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900374?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 2, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96">
+        <v>204168900375</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <v>8</v>
+      </c>
+      <c r="G96">
+        <v>3</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>48</v>
+      </c>
+      <c r="J96">
+        <v>48</v>
+      </c>
+      <c r="K96">
+        <v>48</v>
+      </c>
+      <c r="L96" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900375?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 3, 1, 48, 48, 48);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97">
+        <v>204168900376</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>8</v>
+      </c>
+      <c r="G97">
+        <v>3</v>
+      </c>
+      <c r="H97">
+        <v>2</v>
+      </c>
+      <c r="I97">
+        <v>48</v>
+      </c>
+      <c r="J97">
+        <v>48</v>
+      </c>
+      <c r="K97">
+        <v>48</v>
+      </c>
+      <c r="L97" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into stocking_locations (stocking_location_id, temperature_zone, stocking_location_type, pick_segment, aisle, bay, shelf, shelf_slot, height, width, depth) values ('204168900376?', 'dry'::temperature_zone, 'Pallet Storage'::stocking_location_type, 2, 2, 8, 3, 2, 48, 48, 48);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
routes, tests, and test data for pick_containers, pick_container_locations and pickup_locations
</commit_message>
<xml_diff>
--- a/test_data/generate_sql.xlsx
+++ b/test_data/generate_sql.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="receiving_locations" sheetId="1" r:id="rId1"/>
     <sheet name="stocking_purchase_orders" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="stocking_locations" sheetId="3" r:id="rId3"/>
+    <sheet name="pick_container_locations" sheetId="4" r:id="rId4"/>
+    <sheet name="pick_containers" sheetId="5" r:id="rId5"/>
+    <sheet name="pickup_locations" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="45">
   <si>
     <t>status</t>
   </si>
@@ -94,6 +97,69 @@
   <si>
     <t>depth</t>
   </si>
+  <si>
+    <t>Finished Goods Buffer</t>
+  </si>
+  <si>
+    <t>Pick Cart Parking</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>cold</t>
+  </si>
+  <si>
+    <t>frozen</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>Pick Cart</t>
+  </si>
+  <si>
+    <t>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars)</t>
+  </si>
+  <si>
+    <t>Parking Spot</t>
+  </si>
+  <si>
+    <t>Indoor Pickup Location</t>
+  </si>
+  <si>
+    <t>Lane 1</t>
+  </si>
+  <si>
+    <t>Lane 2</t>
+  </si>
+  <si>
+    <t>Lane 3</t>
+  </si>
+  <si>
+    <t>Lane 4</t>
+  </si>
+  <si>
+    <t>Lane 5</t>
+  </si>
+  <si>
+    <t>Lane 6</t>
+  </si>
+  <si>
+    <t>Lane 7</t>
+  </si>
+  <si>
+    <t>Lane 8</t>
+  </si>
+  <si>
+    <t>Lane 9</t>
+  </si>
+  <si>
+    <t>Lane 10</t>
+  </si>
+  <si>
+    <t>Indoor 1</t>
+  </si>
 </sst>
 </file>
 
@@ -141,8 +207,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -229,7 +325,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -270,6 +366,21 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -310,6 +421,21 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1518,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5315,4 +5441,2791 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>204268900322</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('", A1, "?', '", B1, "', '", C1, "', ", D1, ", ", E1, ", ", F1, ", ", G1, ");")</f>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900322?', 'Finished Goods Buffer', 'cold', 1, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>204268900323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H50" si="0">CONCATENATE("INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('", A2, "?', '", B2, "', '", C2, "', ", D2, ", ", E2, ", ", F2, ", ", G2, ");")</f>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900323?', 'Finished Goods Buffer', 'cold', 1, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>204268900324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900324?', 'Finished Goods Buffer', 'cold', 1, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>204268900325</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900325?', 'Finished Goods Buffer', 'cold', 1, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>204268900326</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900326?', 'Finished Goods Buffer', 'cold', 1, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>204268900327</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900327?', 'Finished Goods Buffer', 'cold', 2, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>204268900328</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900328?', 'Finished Goods Buffer', 'cold', 2, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>204268900329</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900329?', 'Finished Goods Buffer', 'cold', 2, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>204268900330</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900330?', 'Finished Goods Buffer', 'cold', 2, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>204268900331</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900331?', 'Finished Goods Buffer', 'cold', 2, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>204268900332</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900332?', 'Finished Goods Buffer', 'cold', 3, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>204268900333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900333?', 'Finished Goods Buffer', 'cold', 3, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>204268900334</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900334?', 'Finished Goods Buffer', 'cold', 3, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>204268900335</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900335?', 'Finished Goods Buffer', 'cold', 3, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>204268900336</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900336?', 'Finished Goods Buffer', 'cold', 3, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>204268900337</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900337?', 'Finished Goods Buffer', 'frozen', 1, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>204268900338</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900338?', 'Finished Goods Buffer', 'frozen', 1, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>204268900339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900339?', 'Finished Goods Buffer', 'frozen', 1, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>204268900340</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900340?', 'Finished Goods Buffer', 'frozen', 2, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>204268900341</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900341?', 'Finished Goods Buffer', 'frozen', 2, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>204268900342</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900342?', 'Finished Goods Buffer', 'frozen', 2, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>204268900343</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900343?', 'Finished Goods Buffer', 'frozen', 3, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>204268900344</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900344?', 'Finished Goods Buffer', 'frozen', 3, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>204268900345</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900345?', 'Finished Goods Buffer', 'frozen', 3, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>204268900346</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900346?', 'Finished Goods Buffer', 'frozen', 4, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>204268900347</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900347?', 'Pick Cart Parking', 'dry', 1, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>204268900348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900348?', 'Pick Cart Parking', 'dry', 1, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>204268900349</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900349?', 'Pick Cart Parking', 'dry', 1, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>204268900350</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900350?', 'Pick Cart Parking', 'dry', 1, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>204268900351</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900351?', 'Pick Cart Parking', 'dry', 1, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>204268900352</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900352?', 'Pick Cart Parking', 'dry', 2, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>204268900353</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900353?', 'Pick Cart Parking', 'dry', 2, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>204268900354</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900354?', 'Pick Cart Parking', 'dry', 2, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>204268900355</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900355?', 'Pick Cart Parking', 'dry', 2, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>204268900356</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900356?', 'Pick Cart Parking', 'dry', 2, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>204268900357</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900357?', 'Pick Cart Parking', 'dry', 3, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>204268900358</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900358?', 'Pick Cart Parking', 'dry', 3, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>204268900359</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900359?', 'Pick Cart Parking', 'dry', 3, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>204268900360</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900360?', 'Pick Cart Parking', 'dry', 3, 1, 1, 4);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>204268900361</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900361?', 'Pick Cart Parking', 'dry', 3, 1, 1, 5);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>204268900362</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900362?', 'Pick Cart Parking', 'dry', 1, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>204268900363</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900363?', 'Pick Cart Parking', 'dry', 1, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>204268900364</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900364?', 'Pick Cart Parking', 'dry', 1, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>204268900365</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900365?', 'Pick Cart Parking', 'dry', 2, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>204268900366</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900366?', 'Pick Cart Parking', 'dry', 2, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>204268900367</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900367?', 'Pick Cart Parking', 'dry', 2, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>204268900368</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900368?', 'Pick Cart Parking', 'dry', 3, 1, 1, 1);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>204268900369</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900369?', 'Pick Cart Parking', 'dry', 3, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>204268900370</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900370?', 'Pick Cart Parking', 'dry', 3, 1, 1, 3);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>204268900371</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_container_locations (pcl_id, pcl_type, pcl_temperature_zone, pcl_aisle, pcl_bay, pcl_shelf, pcl_shelf_slot) VALUES ('204268900371?', 'Pick Cart Parking', 'dry', 4, 1, 1, 1);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <v>204268900322</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <v>12</v>
+      </c>
+      <c r="F1">
+        <v>18</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('", A1, "?', '",B1, "', '", C1, "', ", D1, ", ", E1, ", ", F1, ");")</f>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900322?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>204268900323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>18</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G50" si="0">CONCATENATE("INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('", A2, "?', '",B2, "', '", C2, "', ", D2, ", ", E2, ", ", F2, ");")</f>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900323?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>204268900324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900324?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>204268900325</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900325?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>204268900326</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900326?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>204268900327</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900327?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>204268900328</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900328?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>204268900329</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900329?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>204268900330</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900330?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>204268900331</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900331?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>204268900332</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>18</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900332?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>204268900333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900333?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>204268900334</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>18</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900334?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>204268900335</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>18</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900335?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>204268900336</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900336?', 'cold', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>204268900337</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>18</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900337?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>204268900338</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>18</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900338?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>204268900339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900339?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>204268900340</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900340?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>204268900341</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900341?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>204268900342</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900342?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>204268900343</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>18</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900343?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>204268900344</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900344?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>204268900345</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>18</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900345?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>204268900346</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>18</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900346?', 'frozen', 'Bin', 18, 12, 18);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>204268900347</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>36</v>
+      </c>
+      <c r="E26">
+        <v>36</v>
+      </c>
+      <c r="F26">
+        <v>18</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900347?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>204268900348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>36</v>
+      </c>
+      <c r="E27">
+        <v>36</v>
+      </c>
+      <c r="F27">
+        <v>18</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900348?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>204268900349</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>36</v>
+      </c>
+      <c r="E28">
+        <v>36</v>
+      </c>
+      <c r="F28">
+        <v>18</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900349?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>204268900350</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>36</v>
+      </c>
+      <c r="F29">
+        <v>18</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900350?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>204268900351</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>36</v>
+      </c>
+      <c r="E30">
+        <v>36</v>
+      </c>
+      <c r="F30">
+        <v>18</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900351?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>204268900352</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>36</v>
+      </c>
+      <c r="E31">
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <v>18</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900352?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>204268900353</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>36</v>
+      </c>
+      <c r="F32">
+        <v>18</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900353?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>204268900354</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>36</v>
+      </c>
+      <c r="F33">
+        <v>18</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900354?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>204268900355</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>36</v>
+      </c>
+      <c r="E34">
+        <v>36</v>
+      </c>
+      <c r="F34">
+        <v>18</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900355?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>204268900356</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>36</v>
+      </c>
+      <c r="E35">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>18</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900356?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>204268900357</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>36</v>
+      </c>
+      <c r="E36">
+        <v>36</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900357?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>204268900358</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>36</v>
+      </c>
+      <c r="E37">
+        <v>36</v>
+      </c>
+      <c r="F37">
+        <v>18</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900358?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>204268900359</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38">
+        <v>36</v>
+      </c>
+      <c r="E38">
+        <v>36</v>
+      </c>
+      <c r="F38">
+        <v>18</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900359?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>204268900360</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>36</v>
+      </c>
+      <c r="E39">
+        <v>36</v>
+      </c>
+      <c r="F39">
+        <v>18</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900360?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>204268900361</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40">
+        <v>36</v>
+      </c>
+      <c r="E40">
+        <v>36</v>
+      </c>
+      <c r="F40">
+        <v>18</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900361?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>204268900362</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>36</v>
+      </c>
+      <c r="E41">
+        <v>36</v>
+      </c>
+      <c r="F41">
+        <v>18</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900362?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>204268900363</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42">
+        <v>36</v>
+      </c>
+      <c r="E42">
+        <v>36</v>
+      </c>
+      <c r="F42">
+        <v>18</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900363?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>204268900364</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>36</v>
+      </c>
+      <c r="E43">
+        <v>36</v>
+      </c>
+      <c r="F43">
+        <v>18</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900364?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>204268900365</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44">
+        <v>36</v>
+      </c>
+      <c r="E44">
+        <v>36</v>
+      </c>
+      <c r="F44">
+        <v>18</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900365?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>204268900366</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>36</v>
+      </c>
+      <c r="E45">
+        <v>36</v>
+      </c>
+      <c r="F45">
+        <v>18</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900366?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>204268900367</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46">
+        <v>36</v>
+      </c>
+      <c r="E46">
+        <v>36</v>
+      </c>
+      <c r="F46">
+        <v>18</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900367?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>204268900368</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <v>36</v>
+      </c>
+      <c r="E47">
+        <v>36</v>
+      </c>
+      <c r="F47">
+        <v>18</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900368?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>204268900369</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48">
+        <v>36</v>
+      </c>
+      <c r="E48">
+        <v>36</v>
+      </c>
+      <c r="F48">
+        <v>18</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900369?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>204268900370</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>36</v>
+      </c>
+      <c r="E49">
+        <v>36</v>
+      </c>
+      <c r="F49">
+        <v>18</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900370?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>204268900371</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50">
+        <v>36</v>
+      </c>
+      <c r="E50">
+        <v>36</v>
+      </c>
+      <c r="F50">
+        <v>18</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pick_containers (pc_id, pc_temperature_zone, pc_type, pc_height, pc_width, pc_depth) VALUES ('204268900371?', 'dry', 'Pick Cart', 36, 36, 18);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('", A1, "', '",B1, "', ", C1, ");")</f>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 1', 0);</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D11" si="0">CONCATENATE("INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('", A2, "', '",B2, "', ", C2, ");")</f>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 2', 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 3', 0);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 4', 0);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 5', 0);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 6', 0);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 7', 0);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 8', 0);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 9', 0);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Parking Spot', 'Lane 10', 0);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pickup_locations (pul_type, pul_display_name, pul_current_cars) VALUES ('Indoor Pickup Location', 'Indoor 1', 0);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>